<commit_message>
major bug fixes with lps
</commit_message>
<xml_diff>
--- a/parts/data/BTC.xlsx
+++ b/parts/data/BTC.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F365"/>
+  <dimension ref="A1:G365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>Volume</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ema</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +491,9 @@
       <c r="F2" t="n">
         <v>24582667004</v>
       </c>
+      <c r="G2" t="n">
+        <v>47686.8125</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -508,6 +516,9 @@
       <c r="F3" t="n">
         <v>27951569547</v>
       </c>
+      <c r="G3" t="n">
+        <v>47601.4140625</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -530,6 +541,9 @@
       <c r="F4" t="n">
         <v>33071628362</v>
       </c>
+      <c r="G4" t="n">
+        <v>47315.58984375</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -552,6 +566,9 @@
       <c r="F5" t="n">
         <v>42494677905</v>
       </c>
+      <c r="G5" t="n">
+        <v>46961.0859375</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -574,6 +591,9 @@
       <c r="F6" t="n">
         <v>36851084859</v>
       </c>
+      <c r="G6" t="n">
+        <v>46113.0654296875</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -596,6 +616,9 @@
       <c r="F7" t="n">
         <v>30208048289</v>
       </c>
+      <c r="G7" t="n">
+        <v>45375.03149414062</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -618,6 +641,9 @@
       <c r="F8" t="n">
         <v>84196607520</v>
       </c>
+      <c r="G8" t="n">
+        <v>44420.74920654297</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -640,6 +666,9 @@
       <c r="F9" t="n">
         <v>28066355845</v>
       </c>
+      <c r="G9" t="n">
+        <v>43749.04725646973</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -662,6 +691,9 @@
       <c r="F10" t="n">
         <v>21294384372</v>
       </c>
+      <c r="G10" t="n">
+        <v>43289.68583297729</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -684,6 +716,9 @@
       <c r="F11" t="n">
         <v>32104232331</v>
       </c>
+      <c r="G11" t="n">
+        <v>42922.57980442047</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -706,6 +741,9 @@
       <c r="F12" t="n">
         <v>26327648900</v>
       </c>
+      <c r="G12" t="n">
+        <v>42875.89872050285</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -728,6 +766,9 @@
       <c r="F13" t="n">
         <v>33499938689</v>
       </c>
+      <c r="G13" t="n">
+        <v>43144.19943100214</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -750,6 +791,9 @@
       <c r="F14" t="n">
         <v>47691135082</v>
       </c>
+      <c r="G14" t="n">
+        <v>43006.04215137661</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -772,6 +816,9 @@
       <c r="F15" t="n">
         <v>23577403399</v>
       </c>
+      <c r="G15" t="n">
+        <v>43029.45641821995</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -794,6 +841,9 @@
       <c r="F16" t="n">
         <v>18371348298</v>
       </c>
+      <c r="G16" t="n">
+        <v>43066.44192303997</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -816,6 +866,9 @@
       <c r="F17" t="n">
         <v>17902097845</v>
       </c>
+      <c r="G17" t="n">
+        <v>43078.30116884247</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -838,6 +891,9 @@
       <c r="F18" t="n">
         <v>21690904261</v>
       </c>
+      <c r="G18" t="n">
+        <v>42871.36357194436</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -860,6 +916,9 @@
       <c r="F19" t="n">
         <v>22417209227</v>
       </c>
+      <c r="G19" t="n">
+        <v>42747.43088208327</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -882,6 +941,9 @@
       <c r="F20" t="n">
         <v>23091543258</v>
       </c>
+      <c r="G20" t="n">
+        <v>42496.65519281245</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -904,6 +966,9 @@
       <c r="F21" t="n">
         <v>20382033940</v>
       </c>
+      <c r="G21" t="n">
+        <v>42042.59588679684</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -926,6 +991,9 @@
       <c r="F22" t="n">
         <v>43011992031</v>
       </c>
+      <c r="G22" t="n">
+        <v>40646.27601666014</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -948,6 +1016,9 @@
       <c r="F23" t="n">
         <v>39714385405</v>
       </c>
+      <c r="G23" t="n">
+        <v>39242.2695124951</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -970,6 +1041,9 @@
       <c r="F24" t="n">
         <v>26017975951</v>
       </c>
+      <c r="G24" t="n">
+        <v>38500.90330624633</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -992,6 +1066,9 @@
       <c r="F25" t="n">
         <v>41856658597</v>
       </c>
+      <c r="G25" t="n">
+        <v>38039.25951093475</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1014,6 +1091,9 @@
       <c r="F26" t="n">
         <v>26428189594</v>
       </c>
+      <c r="G26" t="n">
+        <v>37767.94560976356</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1036,6 +1116,9 @@
       <c r="F27" t="n">
         <v>31324598034</v>
       </c>
+      <c r="G27" t="n">
+        <v>37538.98948076017</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1058,6 +1141,9 @@
       <c r="F28" t="n">
         <v>25041426629</v>
       </c>
+      <c r="G28" t="n">
+        <v>37438.80070432012</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1080,6 +1166,9 @@
       <c r="F29" t="n">
         <v>22238830523</v>
       </c>
+      <c r="G29" t="n">
+        <v>37525.18353605259</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1102,6 +1191,9 @@
       <c r="F30" t="n">
         <v>17194183075</v>
       </c>
+      <c r="G30" t="n">
+        <v>37678.43257391444</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1124,6 +1216,9 @@
       <c r="F31" t="n">
         <v>14643548444</v>
       </c>
+      <c r="G31" t="n">
+        <v>37738.22482106083</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1146,6 +1241,9 @@
       <c r="F32" t="n">
         <v>20734730465</v>
       </c>
+      <c r="G32" t="n">
+        <v>37924.44986579562</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1168,6 +1266,9 @@
       <c r="F33" t="n">
         <v>20288500328</v>
       </c>
+      <c r="G33" t="n">
+        <v>38129.15575872172</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1190,6 +1291,9 @@
       <c r="F34" t="n">
         <v>19155189416</v>
       </c>
+      <c r="G34" t="n">
+        <v>37835.11291279129</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1212,6 +1316,9 @@
       <c r="F35" t="n">
         <v>18591534769</v>
       </c>
+      <c r="G35" t="n">
+        <v>37664.98507521846</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1234,6 +1341,9 @@
       <c r="F36" t="n">
         <v>29412210792</v>
       </c>
+      <c r="G36" t="n">
+        <v>38623.95755641385</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1256,6 +1366,9 @@
       <c r="F37" t="n">
         <v>19652846215</v>
       </c>
+      <c r="G37" t="n">
+        <v>39328.25918293539</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1278,6 +1391,9 @@
       <c r="F38" t="n">
         <v>16142097334</v>
       </c>
+      <c r="G38" t="n">
+        <v>40099.30278563904</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1300,6 +1416,9 @@
       <c r="F39" t="n">
         <v>28641855926</v>
       </c>
+      <c r="G39" t="n">
+        <v>41034.54837829178</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1322,6 +1441,9 @@
       <c r="F40" t="n">
         <v>33079398868</v>
       </c>
+      <c r="G40" t="n">
+        <v>41805.52261184384</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1344,6 +1466,9 @@
       <c r="F41" t="n">
         <v>23245887300</v>
       </c>
+      <c r="G41" t="n">
+        <v>42438.84117763288</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1366,6 +1491,9 @@
       <c r="F42" t="n">
         <v>32142048537</v>
       </c>
+      <c r="G42" t="n">
+        <v>42720.40920353716</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1388,6 +1516,9 @@
       <c r="F43" t="n">
         <v>26954925781</v>
       </c>
+      <c r="G43" t="n">
+        <v>42642.29127765287</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1410,6 +1541,9 @@
       <c r="F44" t="n">
         <v>18152390304</v>
       </c>
+      <c r="G44" t="n">
+        <v>42542.83564573965</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1432,6 +1566,9 @@
       <c r="F45" t="n">
         <v>14741589015</v>
       </c>
+      <c r="G45" t="n">
+        <v>42456.50564055474</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1454,6 +1591,9 @@
       <c r="F46" t="n">
         <v>20827783012</v>
       </c>
+      <c r="G46" t="n">
+        <v>42489.10872260355</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1476,6 +1616,9 @@
       <c r="F47" t="n">
         <v>22721659051</v>
       </c>
+      <c r="G47" t="n">
+        <v>43010.63232320266</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1498,6 +1641,9 @@
       <c r="F48" t="n">
         <v>19792547657</v>
       </c>
+      <c r="G48" t="n">
+        <v>43248.43908615199</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1520,6 +1666,9 @@
       <c r="F49" t="n">
         <v>26246662813</v>
       </c>
+      <c r="G49" t="n">
+        <v>42570.83224430149</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1542,6 +1691,9 @@
       <c r="F50" t="n">
         <v>23310007704</v>
       </c>
+      <c r="G50" t="n">
+        <v>41935.86832385111</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1564,6 +1716,9 @@
       <c r="F51" t="n">
         <v>13736557863</v>
       </c>
+      <c r="G51" t="n">
+        <v>41482.44030538834</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1586,6 +1741,9 @@
       <c r="F52" t="n">
         <v>18340576452</v>
       </c>
+      <c r="G52" t="n">
+        <v>40719.67495560375</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1608,6 +1766,9 @@
       <c r="F53" t="n">
         <v>29280402798</v>
       </c>
+      <c r="G53" t="n">
+        <v>39808.57652920282</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1630,6 +1791,9 @@
       <c r="F54" t="n">
         <v>25493150450</v>
       </c>
+      <c r="G54" t="n">
+        <v>39427.93923283961</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1652,6 +1816,9 @@
       <c r="F55" t="n">
         <v>21849073843</v>
       </c>
+      <c r="G55" t="n">
+        <v>38895.09700275471</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1674,6 +1841,9 @@
       <c r="F56" t="n">
         <v>46383802093</v>
       </c>
+      <c r="G56" t="n">
+        <v>38754.47509581603</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1696,6 +1866,9 @@
       <c r="F57" t="n">
         <v>26545599159</v>
       </c>
+      <c r="G57" t="n">
+        <v>38869.41100936203</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1718,6 +1891,9 @@
       <c r="F58" t="n">
         <v>17467554129</v>
       </c>
+      <c r="G58" t="n">
+        <v>38928.34536639652</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1740,6 +1916,9 @@
       <c r="F59" t="n">
         <v>23450127612</v>
       </c>
+      <c r="G59" t="n">
+        <v>38623.70531385989</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1762,6 +1941,9 @@
       <c r="F60" t="n">
         <v>35690014104</v>
       </c>
+      <c r="G60" t="n">
+        <v>39766.08757914491</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1784,6 +1966,9 @@
       <c r="F61" t="n">
         <v>32479047645</v>
       </c>
+      <c r="G61" t="n">
+        <v>40913.22486404618</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1806,6 +1991,9 @@
       <c r="F62" t="n">
         <v>29183112630</v>
       </c>
+      <c r="G62" t="n">
+        <v>41665.94794490964</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1828,6 +2016,9 @@
       <c r="F63" t="n">
         <v>24967782593</v>
       </c>
+      <c r="G63" t="n">
+        <v>41862.40822430723</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1850,6 +2041,9 @@
       <c r="F64" t="n">
         <v>28516271427</v>
       </c>
+      <c r="G64" t="n">
+        <v>41181.20753541793</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1872,6 +2066,9 @@
       <c r="F65" t="n">
         <v>16975917450</v>
       </c>
+      <c r="G65" t="n">
+        <v>40736.05213593844</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1894,6 +2091,9 @@
       <c r="F66" t="n">
         <v>19745229902</v>
       </c>
+      <c r="G66" t="n">
+        <v>40157.03519570384</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1916,6 +2116,9 @@
       <c r="F67" t="n">
         <v>28546143503</v>
       </c>
+      <c r="G67" t="n">
+        <v>39633.28616240287</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1938,6 +2141,9 @@
       <c r="F68" t="n">
         <v>25776583476</v>
       </c>
+      <c r="G68" t="n">
+        <v>39409.28200461465</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1960,6 +2166,9 @@
       <c r="F69" t="n">
         <v>32284121034</v>
       </c>
+      <c r="G69" t="n">
+        <v>40052.69294877349</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1982,6 +2191,9 @@
       <c r="F70" t="n">
         <v>31078064711</v>
       </c>
+      <c r="G70" t="n">
+        <v>39898.88494595511</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2004,6 +2216,9 @@
       <c r="F71" t="n">
         <v>26364890465</v>
       </c>
+      <c r="G71" t="n">
+        <v>39622.90687352883</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2026,6 +2241,9 @@
       <c r="F72" t="n">
         <v>14616450657</v>
       </c>
+      <c r="G72" t="n">
+        <v>39443.18308483412</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2048,6 +2266,9 @@
       <c r="F73" t="n">
         <v>17300745310</v>
       </c>
+      <c r="G73" t="n">
+        <v>39044.80332925059</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2070,6 +2291,9 @@
       <c r="F74" t="n">
         <v>24322159070</v>
       </c>
+      <c r="G74" t="n">
+        <v>39200.29097350044</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2092,6 +2316,9 @@
       <c r="F75" t="n">
         <v>23934000868</v>
       </c>
+      <c r="G75" t="n">
+        <v>39234.91451918783</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2114,6 +2341,9 @@
       <c r="F76" t="n">
         <v>39616916192</v>
       </c>
+      <c r="G76" t="n">
+        <v>39712.16831126587</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2136,6 +2366,9 @@
       <c r="F77" t="n">
         <v>22009601093</v>
       </c>
+      <c r="G77" t="n">
+        <v>40021.9709600119</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2158,6 +2391,9 @@
       <c r="F78" t="n">
         <v>34421564942</v>
       </c>
+      <c r="G78" t="n">
+        <v>40466.76728250892</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2180,6 +2416,9 @@
       <c r="F79" t="n">
         <v>19664853187</v>
       </c>
+      <c r="G79" t="n">
+        <v>40897.73854781919</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2202,6 +2441,9 @@
       <c r="F80" t="n">
         <v>20127946682</v>
       </c>
+      <c r="G80" t="n">
+        <v>40985.25996555189</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2224,6 +2466,9 @@
       <c r="F81" t="n">
         <v>24615543271</v>
       </c>
+      <c r="G81" t="n">
+        <v>41008.44399760142</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2246,6 +2491,9 @@
       <c r="F82" t="n">
         <v>32004652376</v>
       </c>
+      <c r="G82" t="n">
+        <v>41346.03514663856</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2268,6 +2516,9 @@
       <c r="F83" t="n">
         <v>25242943069</v>
       </c>
+      <c r="G83" t="n">
+        <v>41732.76561779142</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2290,6 +2541,9 @@
       <c r="F84" t="n">
         <v>31042992291</v>
       </c>
+      <c r="G84" t="n">
+        <v>42289.80761178106</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2312,6 +2566,9 @@
       <c r="F85" t="n">
         <v>30574413034</v>
       </c>
+      <c r="G85" t="n">
+        <v>42804.5383260233</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2334,6 +2591,9 @@
       <c r="F86" t="n">
         <v>16950455995</v>
       </c>
+      <c r="G86" t="n">
+        <v>43228.61077576748</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2356,6 +2616,9 @@
       <c r="F87" t="n">
         <v>28160889722</v>
       </c>
+      <c r="G87" t="n">
+        <v>44126.58112870061</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2378,6 +2641,9 @@
       <c r="F88" t="n">
         <v>36362175703</v>
       </c>
+      <c r="G88" t="n">
+        <v>44876.93682308796</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2400,6 +2666,9 @@
       <c r="F89" t="n">
         <v>31397059069</v>
       </c>
+      <c r="G89" t="n">
+        <v>45524.13523450347</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2422,6 +2691,9 @@
       <c r="F90" t="n">
         <v>29333883962</v>
       </c>
+      <c r="G90" t="n">
+        <v>45908.7674415026</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2444,6 +2716,9 @@
       <c r="F91" t="n">
         <v>33327427106</v>
       </c>
+      <c r="G91" t="n">
+        <v>45816.24452643945</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2466,6 +2741,9 @@
       <c r="F92" t="n">
         <v>38162644287</v>
       </c>
+      <c r="G92" t="n">
+        <v>45932.59452764208</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2488,6 +2766,9 @@
       <c r="F93" t="n">
         <v>29336594194</v>
       </c>
+      <c r="G93" t="n">
+        <v>45916.68320041907</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2510,6 +2791,9 @@
       <c r="F94" t="n">
         <v>25414397610</v>
       </c>
+      <c r="G94" t="n">
+        <v>46050.9040018768</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2532,6 +2816,9 @@
       <c r="F95" t="n">
         <v>32499785455</v>
       </c>
+      <c r="G95" t="n">
+        <v>46193.8469467201</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2554,6 +2841,9 @@
       <c r="F96" t="n">
         <v>29640604055</v>
       </c>
+      <c r="G96" t="n">
+        <v>46034.38325691508</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2576,6 +2866,9 @@
       <c r="F97" t="n">
         <v>39393395788</v>
       </c>
+      <c r="G97" t="n">
+        <v>45327.47201299881</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2598,6 +2891,9 @@
       <c r="F98" t="n">
         <v>26101973106</v>
       </c>
+      <c r="G98" t="n">
+        <v>44871.56592381161</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2620,6 +2916,9 @@
       <c r="F99" t="n">
         <v>27215995394</v>
       </c>
+      <c r="G99" t="n">
+        <v>44225.5904584837</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2642,6 +2941,9 @@
       <c r="F100" t="n">
         <v>16050772496</v>
       </c>
+      <c r="G100" t="n">
+        <v>43864.72702355028</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2664,6 +2966,9 @@
       <c r="F101" t="n">
         <v>17654475582</v>
       </c>
+      <c r="G101" t="n">
+        <v>43450.46323641271</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2686,6 +2991,9 @@
       <c r="F102" t="n">
         <v>33949912166</v>
       </c>
+      <c r="G102" t="n">
+        <v>42468.32301324703</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2708,6 +3016,9 @@
       <c r="F103" t="n">
         <v>30991500854</v>
       </c>
+      <c r="G103" t="n">
+        <v>41883.03815837277</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2730,6 +3041,9 @@
       <c r="F104" t="n">
         <v>27691105228</v>
       </c>
+      <c r="G104" t="n">
+        <v>41703.96123596708</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2752,6 +3066,9 @@
       <c r="F105" t="n">
         <v>24342001973</v>
       </c>
+      <c r="G105" t="n">
+        <v>41261.84983322531</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2774,6 +3091,9 @@
       <c r="F106" t="n">
         <v>21756855753</v>
       </c>
+      <c r="G106" t="n">
+        <v>41084.75358585648</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2796,6 +3116,9 @@
       <c r="F107" t="n">
         <v>16833150693</v>
       </c>
+      <c r="G107" t="n">
+        <v>40919.68628314236</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2818,6 +3141,9 @@
       <c r="F108" t="n">
         <v>19087633042</v>
       </c>
+      <c r="G108" t="n">
+        <v>40619.00299360677</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2840,6 +3166,9 @@
       <c r="F109" t="n">
         <v>33705182072</v>
       </c>
+      <c r="G109" t="n">
+        <v>40670.80595614258</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2862,6 +3191,9 @@
       <c r="F110" t="n">
         <v>25303206547</v>
       </c>
+      <c r="G110" t="n">
+        <v>40878.79196710693</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2884,6 +3216,9 @@
       <c r="F111" t="n">
         <v>27819532341</v>
       </c>
+      <c r="G111" t="n">
+        <v>41002.6887018927</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2906,6 +3241,9 @@
       <c r="F112" t="n">
         <v>35372786395</v>
       </c>
+      <c r="G112" t="n">
+        <v>40883.85734673202</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2928,6 +3266,9 @@
       <c r="F113" t="n">
         <v>28011716745</v>
       </c>
+      <c r="G113" t="n">
+        <v>40597.97308817402</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2950,6 +3291,9 @@
       <c r="F114" t="n">
         <v>16138021249</v>
       </c>
+      <c r="G114" t="n">
+        <v>40320.16243331802</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2972,6 +3316,9 @@
       <c r="F115" t="n">
         <v>17964398167</v>
       </c>
+      <c r="G115" t="n">
+        <v>40107.44506717601</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2994,6 +3341,9 @@
       <c r="F116" t="n">
         <v>35445730570</v>
       </c>
+      <c r="G116" t="n">
+        <v>40195.16094881951</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3016,6 +3366,9 @@
       <c r="F117" t="n">
         <v>34569088416</v>
       </c>
+      <c r="G117" t="n">
+        <v>39675.73594598963</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3038,6 +3391,9 @@
       <c r="F118" t="n">
         <v>30981015184</v>
       </c>
+      <c r="G118" t="n">
+        <v>39567.08223292972</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3060,6 +3416,9 @@
       <c r="F119" t="n">
         <v>33903704907</v>
       </c>
+      <c r="G119" t="n">
+        <v>39618.7687059473</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3082,6 +3441,9 @@
       <c r="F120" t="n">
         <v>30882994649</v>
       </c>
+      <c r="G120" t="n">
+        <v>39366.53258414797</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3104,6 +3466,9 @@
       <c r="F121" t="n">
         <v>23895713731</v>
       </c>
+      <c r="G121" t="n">
+        <v>38953.61818811098</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3126,6 +3491,9 @@
       <c r="F122" t="n">
         <v>27002760110</v>
       </c>
+      <c r="G122" t="n">
+        <v>38832.48707858323</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3148,6 +3516,9 @@
       <c r="F123" t="n">
         <v>32922642426</v>
       </c>
+      <c r="G123" t="n">
+        <v>38756.69734018743</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3170,6 +3541,9 @@
       <c r="F124" t="n">
         <v>27326943244</v>
       </c>
+      <c r="G124" t="n">
+        <v>38505.13628639057</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3192,6 +3566,9 @@
       <c r="F125" t="n">
         <v>36754404490</v>
       </c>
+      <c r="G125" t="n">
+        <v>38803.44498823043</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3214,6 +3591,9 @@
       <c r="F126" t="n">
         <v>43106256317</v>
       </c>
+      <c r="G126" t="n">
+        <v>38246.36889742282</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3236,6 +3616,9 @@
       <c r="F127" t="n">
         <v>37795577489</v>
       </c>
+      <c r="G127" t="n">
+        <v>37695.00714181711</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3258,6 +3641,9 @@
       <c r="F128" t="n">
         <v>24375896406</v>
       </c>
+      <c r="G128" t="n">
+        <v>37146.74363761283</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3280,6 +3666,9 @@
       <c r="F129" t="n">
         <v>36763041910</v>
       </c>
+      <c r="G129" t="n">
+        <v>36374.87413445962</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3302,6 +3691,9 @@
       <c r="F130" t="n">
         <v>63355494961</v>
       </c>
+      <c r="G130" t="n">
+        <v>34855.39388209472</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3324,6 +3716,9 @@
       <c r="F131" t="n">
         <v>59811038817</v>
       </c>
+      <c r="G131" t="n">
+        <v>33897.27197407104</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3346,6 +3741,9 @@
       <c r="F132" t="n">
         <v>70388855818</v>
       </c>
+      <c r="G132" t="n">
+        <v>32657.04284774078</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3368,6 +3766,9 @@
       <c r="F133" t="n">
         <v>66989173272</v>
       </c>
+      <c r="G133" t="n">
+        <v>31754.72012408683</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3390,6 +3791,9 @@
       <c r="F134" t="n">
         <v>42841124537</v>
       </c>
+      <c r="G134" t="n">
+        <v>31136.81597197137</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3412,6 +3816,9 @@
       <c r="F135" t="n">
         <v>28579868620</v>
       </c>
+      <c r="G135" t="n">
+        <v>30877.92838522853</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3434,6 +3841,9 @@
       <c r="F136" t="n">
         <v>25835372065</v>
       </c>
+      <c r="G136" t="n">
+        <v>30984.7246092339</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3456,6 +3866,9 @@
       <c r="F137" t="n">
         <v>32613897286</v>
       </c>
+      <c r="G137" t="n">
+        <v>30704.27294911292</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3478,6 +3891,9 @@
       <c r="F138" t="n">
         <v>29101473475</v>
       </c>
+      <c r="G138" t="n">
+        <v>30634.66906730344</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3500,6 +3916,9 @@
       <c r="F139" t="n">
         <v>31285268319</v>
       </c>
+      <c r="G139" t="n">
+        <v>30156.06967157133</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3522,6 +3941,9 @@
       <c r="F140" t="n">
         <v>33773447707</v>
       </c>
+      <c r="G140" t="n">
+        <v>30195.63574977225</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3544,6 +3966,9 @@
       <c r="F141" t="n">
         <v>30749382605</v>
       </c>
+      <c r="G141" t="n">
+        <v>29946.91187092293</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -3566,6 +3991,9 @@
       <c r="F142" t="n">
         <v>17274840442</v>
       </c>
+      <c r="G142" t="n">
+        <v>29818.2405438172</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -3588,6 +4016,9 @@
       <c r="F143" t="n">
         <v>21631532270</v>
       </c>
+      <c r="G143" t="n">
+        <v>29944.6110719254</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -3610,6 +4041,9 @@
       <c r="F144" t="n">
         <v>31483454557</v>
       </c>
+      <c r="G144" t="n">
+        <v>29733.18584300655</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -3632,6 +4066,9 @@
       <c r="F145" t="n">
         <v>26616506245</v>
       </c>
+      <c r="G145" t="n">
+        <v>29713.78586662991</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -3654,6 +4091,9 @@
       <c r="F146" t="n">
         <v>27525063551</v>
       </c>
+      <c r="G146" t="n">
+        <v>29675.92973200368</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -3676,6 +4116,9 @@
       <c r="F147" t="n">
         <v>36774325352</v>
       </c>
+      <c r="G147" t="n">
+        <v>29573.75345134651</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -3698,6 +4141,9 @@
       <c r="F148" t="n">
         <v>36582005748</v>
       </c>
+      <c r="G148" t="n">
+        <v>29337.20864319738</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -3720,6 +4166,9 @@
       <c r="F149" t="n">
         <v>35519577634</v>
       </c>
+      <c r="G149" t="n">
+        <v>29206.63158005429</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -3742,6 +4191,9 @@
       <c r="F150" t="n">
         <v>18093886409</v>
       </c>
+      <c r="G150" t="n">
+        <v>29266.46294285321</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -3764,6 +4216,9 @@
       <c r="F151" t="n">
         <v>39277993274</v>
       </c>
+      <c r="G151" t="n">
+        <v>29881.44486338991</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3786,6 +4241,9 @@
       <c r="F152" t="n">
         <v>33538210634</v>
       </c>
+      <c r="G152" t="n">
+        <v>30359.16128426118</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -3808,6 +4266,9 @@
       <c r="F153" t="n">
         <v>41135817341</v>
       </c>
+      <c r="G153" t="n">
+        <v>30219.14098272713</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -3830,6 +4291,9 @@
       <c r="F154" t="n">
         <v>29083562061</v>
       </c>
+      <c r="G154" t="n">
+        <v>30281.22780735785</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -3852,6 +4316,9 @@
       <c r="F155" t="n">
         <v>26175547452</v>
       </c>
+      <c r="G155" t="n">
+        <v>30137.01851176839</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -3874,6 +4341,9 @@
       <c r="F156" t="n">
         <v>16588370958</v>
       </c>
+      <c r="G156" t="n">
+        <v>30060.99239945129</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3896,6 +4366,9 @@
       <c r="F157" t="n">
         <v>17264085441</v>
       </c>
+      <c r="G157" t="n">
+        <v>30022.40982693222</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -3918,6 +4391,9 @@
       <c r="F158" t="n">
         <v>31947336829</v>
       </c>
+      <c r="G158" t="n">
+        <v>30359.47533894916</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3940,6 +4416,9 @@
       <c r="F159" t="n">
         <v>40770974039</v>
       </c>
+      <c r="G159" t="n">
+        <v>30558.47613311812</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -3962,6 +4441,9 @@
       <c r="F160" t="n">
         <v>30242059107</v>
       </c>
+      <c r="G160" t="n">
+        <v>30472.44596702609</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -3984,6 +4466,9 @@
       <c r="F161" t="n">
         <v>21692004719</v>
       </c>
+      <c r="G161" t="n">
+        <v>30382.33398698832</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -4006,6 +4491,9 @@
       <c r="F162" t="n">
         <v>29867476527</v>
       </c>
+      <c r="G162" t="n">
+        <v>30057.70166211624</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -4028,6 +4516,9 @@
       <c r="F163" t="n">
         <v>27246574439</v>
       </c>
+      <c r="G163" t="n">
+        <v>29633.47888330593</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -4050,6 +4541,9 @@
       <c r="F164" t="n">
         <v>34163220274</v>
       </c>
+      <c r="G164" t="n">
+        <v>28915.77127185445</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -4072,6 +4566,9 @@
       <c r="F165" t="n">
         <v>68204556440</v>
       </c>
+      <c r="G165" t="n">
+        <v>27308.67562185958</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -4094,6 +4591,9 @@
       <c r="F166" t="n">
         <v>50913575242</v>
       </c>
+      <c r="G166" t="n">
+        <v>26033.20495858219</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -4116,6 +4616,9 @@
       <c r="F167" t="n">
         <v>54912007015</v>
       </c>
+      <c r="G167" t="n">
+        <v>25168.11367987414</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -4138,6 +4641,9 @@
       <c r="F168" t="n">
         <v>31183975654</v>
       </c>
+      <c r="G168" t="n">
+        <v>23971.49785756186</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -4160,6 +4666,9 @@
       <c r="F169" t="n">
         <v>27132421514</v>
       </c>
+      <c r="G169" t="n">
+        <v>23096.49399864014</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -4182,6 +4691,9 @@
       <c r="F170" t="n">
         <v>42009436760</v>
       </c>
+      <c r="G170" t="n">
+        <v>22076.78114351136</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -4204,6 +4716,9 @@
       <c r="F171" t="n">
         <v>35329942625</v>
       </c>
+      <c r="G171" t="n">
+        <v>21695.90372872727</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -4226,6 +4741,9 @@
       <c r="F172" t="n">
         <v>30818458597</v>
       </c>
+      <c r="G172" t="n">
+        <v>21421.8120738892</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -4248,6 +4766,9 @@
       <c r="F173" t="n">
         <v>28970212744</v>
       </c>
+      <c r="G173" t="n">
+        <v>21244.0084694794</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -4270,6 +4791,9 @@
       <c r="F174" t="n">
         <v>28574793478</v>
       </c>
+      <c r="G174" t="n">
+        <v>20929.7636763283</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -4292,6 +4816,9 @@
       <c r="F175" t="n">
         <v>26188097173</v>
       </c>
+      <c r="G175" t="n">
+        <v>20968.79199552748</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -4314,6 +4841,9 @@
       <c r="F176" t="n">
         <v>24957784918</v>
       </c>
+      <c r="G176" t="n">
+        <v>21034.50805914561</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -4336,6 +4866,9 @@
       <c r="F177" t="n">
         <v>18372538715</v>
       </c>
+      <c r="G177" t="n">
+        <v>21151.46551701545</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -4358,6 +4891,9 @@
       <c r="F178" t="n">
         <v>18027170497</v>
       </c>
+      <c r="G178" t="n">
+        <v>21120.42286823034</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -4380,6 +4916,9 @@
       <c r="F179" t="n">
         <v>20965695707</v>
       </c>
+      <c r="G179" t="n">
+        <v>21024.18678007901</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -4402,6 +4941,9 @@
       <c r="F180" t="n">
         <v>21381535161</v>
       </c>
+      <c r="G180" t="n">
+        <v>20838.2987764655</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -4424,6 +4966,9 @@
       <c r="F181" t="n">
         <v>23552740328</v>
       </c>
+      <c r="G181" t="n">
+        <v>20654.72994172413</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -4446,6 +4991,9 @@
       <c r="F182" t="n">
         <v>26267239923</v>
       </c>
+      <c r="G182" t="n">
+        <v>20437.2290969181</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -4468,6 +5016,9 @@
       <c r="F183" t="n">
         <v>30767551159</v>
       </c>
+      <c r="G183" t="n">
+        <v>20145.26361956357</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -4490,6 +5041,9 @@
       <c r="F184" t="n">
         <v>18100418740</v>
       </c>
+      <c r="G184" t="n">
+        <v>19919.51167951643</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -4512,6 +5066,9 @@
       <c r="F185" t="n">
         <v>16390821947</v>
       </c>
+      <c r="G185" t="n">
+        <v>19763.90280260607</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -4534,6 +5091,9 @@
       <c r="F186" t="n">
         <v>21594638208</v>
       </c>
+      <c r="G186" t="n">
+        <v>19880.74253164205</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -4556,6 +5116,9 @@
       <c r="F187" t="n">
         <v>26715546990</v>
       </c>
+      <c r="G187" t="n">
+        <v>19958.08570732529</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -4578,6 +5141,9 @@
       <c r="F188" t="n">
         <v>24598943708</v>
       </c>
+      <c r="G188" t="n">
+        <v>20105.62580393147</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -4600,6 +5166,9 @@
       <c r="F189" t="n">
         <v>25814972520</v>
       </c>
+      <c r="G189" t="n">
+        <v>20488.61632560485</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -4622,6 +5191,9 @@
       <c r="F190" t="n">
         <v>49899834488</v>
       </c>
+      <c r="G190" t="n">
+        <v>20799.24154107864</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -4644,6 +5216,9 @@
       <c r="F191" t="n">
         <v>29641127858</v>
       </c>
+      <c r="G191" t="n">
+        <v>20997.48291362148</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -4666,6 +5241,9 @@
       <c r="F192" t="n">
         <v>28688807249</v>
       </c>
+      <c r="G192" t="n">
+        <v>20963.22448990361</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -4688,6 +5266,9 @@
       <c r="F193" t="n">
         <v>24150249025</v>
       </c>
+      <c r="G193" t="n">
+        <v>20715.05752758396</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -4710,6 +5291,9 @@
       <c r="F194" t="n">
         <v>25810220018</v>
       </c>
+      <c r="G194" t="n">
+        <v>20367.27166131297</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -4732,6 +5316,9 @@
       <c r="F195" t="n">
         <v>33042430345</v>
       </c>
+      <c r="G195" t="n">
+        <v>20328.47230067223</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -4754,6 +5341,9 @@
       <c r="F196" t="n">
         <v>31158743333</v>
       </c>
+      <c r="G196" t="n">
+        <v>20388.83420597292</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -4776,6 +5366,9 @@
       <c r="F197" t="n">
         <v>25905575359</v>
       </c>
+      <c r="G197" t="n">
+        <v>20500.70768572969</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -4798,6 +5391,9 @@
       <c r="F198" t="n">
         <v>24302954056</v>
       </c>
+      <c r="G198" t="n">
+        <v>20673.10986585977</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -4820,6 +5416,9 @@
       <c r="F199" t="n">
         <v>22927802083</v>
       </c>
+      <c r="G199" t="n">
+        <v>20699.66833689483</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -4842,6 +5441,9 @@
       <c r="F200" t="n">
         <v>39974475562</v>
       </c>
+      <c r="G200" t="n">
+        <v>21146.17361595237</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -4864,6 +5466,9 @@
       <c r="F201" t="n">
         <v>48765202697</v>
       </c>
+      <c r="G201" t="n">
+        <v>21706.98861040178</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -4886,6 +5491,9 @@
       <c r="F202" t="n">
         <v>42932549127</v>
       </c>
+      <c r="G202" t="n">
+        <v>22088.17456327008</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -4908,6 +5516,9 @@
       <c r="F203" t="n">
         <v>33631012204</v>
       </c>
+      <c r="G203" t="n">
+        <v>22357.28814901506</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -4930,6 +5541,9 @@
       <c r="F204" t="n">
         <v>31421555646</v>
       </c>
+      <c r="G204" t="n">
+        <v>22446.71074066755</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -4952,6 +5566,9 @@
       <c r="F205" t="n">
         <v>24021799169</v>
       </c>
+      <c r="G205" t="n">
+        <v>22451.40268440691</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -4974,6 +5591,9 @@
       <c r="F206" t="n">
         <v>23565495303</v>
       </c>
+      <c r="G206" t="n">
+        <v>22490.84302893018</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -4996,6 +5616,9 @@
       <c r="F207" t="n">
         <v>35574561406</v>
       </c>
+      <c r="G207" t="n">
+        <v>22208.55756466639</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -5018,6 +5641,9 @@
       <c r="F208" t="n">
         <v>28624673855</v>
       </c>
+      <c r="G208" t="n">
+        <v>21966.35665006229</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -5040,6 +5666,9 @@
       <c r="F209" t="n">
         <v>31758955233</v>
       </c>
+      <c r="G209" t="n">
+        <v>22207.40469457797</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -5062,6 +5691,9 @@
       <c r="F210" t="n">
         <v>40212386158</v>
       </c>
+      <c r="G210" t="n">
+        <v>22616.52520062098</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -5084,6 +5716,9 @@
       <c r="F211" t="n">
         <v>35887249746</v>
       </c>
+      <c r="G211" t="n">
+        <v>22913.55210359073</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -5106,6 +5741,9 @@
       <c r="F212" t="n">
         <v>28148218301</v>
       </c>
+      <c r="G212" t="n">
+        <v>23099.21583550555</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -5128,6 +5766,9 @@
       <c r="F213" t="n">
         <v>23553591896</v>
       </c>
+      <c r="G213" t="n">
+        <v>23158.63599772291</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -5150,6 +5791,9 @@
       <c r="F214" t="n">
         <v>25849159141</v>
       </c>
+      <c r="G214" t="n">
+        <v>23197.52680297969</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -5172,6 +5816,9 @@
       <c r="F215" t="n">
         <v>28389250717</v>
       </c>
+      <c r="G215" t="n">
+        <v>23142.67439910976</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -5194,6 +5841,9 @@
       <c r="F216" t="n">
         <v>26288169966</v>
       </c>
+      <c r="G216" t="n">
+        <v>23068.63275245732</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -5216,6 +5866,9 @@
       <c r="F217" t="n">
         <v>25120229769</v>
       </c>
+      <c r="G217" t="n">
+        <v>22959.21382215549</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -5238,6 +5891,9 @@
       <c r="F218" t="n">
         <v>28881249043</v>
       </c>
+      <c r="G218" t="n">
+        <v>23041.73897989787</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -5260,6 +5916,9 @@
       <c r="F219" t="n">
         <v>15978259885</v>
       </c>
+      <c r="G219" t="n">
+        <v>23021.62405914215</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -5282,6 +5941,9 @@
       <c r="F220" t="n">
         <v>15886817043</v>
       </c>
+      <c r="G220" t="n">
+        <v>23060.19070060661</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -5304,6 +5966,9 @@
       <c r="F221" t="n">
         <v>28575544847</v>
       </c>
+      <c r="G221" t="n">
+        <v>23247.51460748621</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -5326,6 +5991,9 @@
       <c r="F222" t="n">
         <v>23555719219</v>
       </c>
+      <c r="G222" t="n">
+        <v>23226.71554545841</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -5348,6 +6016,9 @@
       <c r="F223" t="n">
         <v>32837431722</v>
       </c>
+      <c r="G223" t="n">
+        <v>23406.94730362506</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -5370,6 +6041,9 @@
       <c r="F224" t="n">
         <v>37127036580</v>
       </c>
+      <c r="G224" t="n">
+        <v>23544.59280193754</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -5392,6 +6066,9 @@
       <c r="F225" t="n">
         <v>27265804688</v>
       </c>
+      <c r="G225" t="n">
+        <v>23759.14919129691</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -5414,6 +6091,9 @@
       <c r="F226" t="n">
         <v>22987346289</v>
       </c>
+      <c r="G226" t="n">
+        <v>23925.37898331643</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -5436,6 +6116,9 @@
       <c r="F227" t="n">
         <v>22994133555</v>
       </c>
+      <c r="G227" t="n">
+        <v>24023.86773358107</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -5458,6 +6141,9 @@
       <c r="F228" t="n">
         <v>35123501685</v>
       </c>
+      <c r="G228" t="n">
+        <v>24052.1439642483</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -5480,6 +6166,9 @@
       <c r="F229" t="n">
         <v>27753685646</v>
       </c>
+      <c r="G229" t="n">
+        <v>24009.93072709248</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -5502,6 +6191,9 @@
       <c r="F230" t="n">
         <v>30931623076</v>
       </c>
+      <c r="G230" t="n">
+        <v>23841.44755703811</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -5524,6 +6216,9 @@
       <c r="F231" t="n">
         <v>23747613147</v>
       </c>
+      <c r="G231" t="n">
+        <v>23684.27023809108</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -5546,6 +6241,9 @@
       <c r="F232" t="n">
         <v>40509610260</v>
       </c>
+      <c r="G232" t="n">
+        <v>22982.59086216206</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -5568,6 +6266,9 @@
       <c r="F233" t="n">
         <v>27595671000</v>
       </c>
+      <c r="G233" t="n">
+        <v>22528.4582833403</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -5590,6 +6291,9 @@
       <c r="F234" t="n">
         <v>23102307723</v>
       </c>
+      <c r="G234" t="n">
+        <v>22279.87398594272</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -5612,6 +6316,9 @@
       <c r="F235" t="n">
         <v>31666498758</v>
       </c>
+      <c r="G235" t="n">
+        <v>22059.63254023829</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -5634,6 +6341,9 @@
       <c r="F236" t="n">
         <v>31878280659</v>
       </c>
+      <c r="G236" t="n">
+        <v>21926.74637783497</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -5656,6 +6366,9 @@
       <c r="F237" t="n">
         <v>31962253368</v>
       </c>
+      <c r="G237" t="n">
+        <v>21793.81466618873</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -5678,6 +6391,9 @@
       <c r="F238" t="n">
         <v>31028679593</v>
       </c>
+      <c r="G238" t="n">
+        <v>21745.5870738603</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -5700,6 +6416,9 @@
       <c r="F239" t="n">
         <v>42326789564</v>
       </c>
+      <c r="G239" t="n">
+        <v>21374.19518820772</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -5722,6 +6441,9 @@
       <c r="F240" t="n">
         <v>30116729776</v>
       </c>
+      <c r="G240" t="n">
+        <v>21041.08096146829</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -5744,6 +6466,9 @@
       <c r="F241" t="n">
         <v>24366810591</v>
       </c>
+      <c r="G241" t="n">
+        <v>20685.01433438247</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -5766,6 +6491,9 @@
       <c r="F242" t="n">
         <v>32637854078</v>
       </c>
+      <c r="G242" t="n">
+        <v>20588.2592859431</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -5788,6 +6516,9 @@
       <c r="F243" t="n">
         <v>34483360283</v>
       </c>
+      <c r="G243" t="n">
+        <v>20390.39661289483</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -5810,6 +6541,9 @@
       <c r="F244" t="n">
         <v>33225232872</v>
       </c>
+      <c r="G244" t="n">
+        <v>20305.23837763987</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -5832,6 +6566,9 @@
       <c r="F245" t="n">
         <v>30182031010</v>
       </c>
+      <c r="G245" t="n">
+        <v>20260.7139394799</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -5854,6 +6591,9 @@
       <c r="F246" t="n">
         <v>29123998928</v>
       </c>
+      <c r="G246" t="n">
+        <v>20187.97832570368</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -5876,6 +6616,9 @@
       <c r="F247" t="n">
         <v>23613051457</v>
       </c>
+      <c r="G247" t="n">
+        <v>20099.00571693401</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -5898,6 +6641,9 @@
       <c r="F248" t="n">
         <v>25245861652</v>
       </c>
+      <c r="G248" t="n">
+        <v>20070.93251035675</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -5920,6 +6666,9 @@
       <c r="F249" t="n">
         <v>28813460025</v>
       </c>
+      <c r="G249" t="n">
+        <v>20006.29215620507</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -5942,6 +6691,9 @@
       <c r="F250" t="n">
         <v>43403978910</v>
       </c>
+      <c r="G250" t="n">
+        <v>19714.1361093413</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -5964,6 +6716,9 @@
       <c r="F251" t="n">
         <v>35239757134</v>
       </c>
+      <c r="G251" t="n">
+        <v>19608.18313669347</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -5986,6 +6741,9 @@
       <c r="F252" t="n">
         <v>32194477850</v>
       </c>
+      <c r="G252" t="n">
+        <v>19538.59584861386</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -6008,6 +6766,9 @@
       <c r="F253" t="n">
         <v>48469528171</v>
       </c>
+      <c r="G253" t="n">
+        <v>19999.23497239789</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -6030,6 +6791,9 @@
       <c r="F254" t="n">
         <v>36913738894</v>
       </c>
+      <c r="G254" t="n">
+        <v>20419.56099492342</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -6052,6 +6816,9 @@
       <c r="F255" t="n">
         <v>34493951963</v>
       </c>
+      <c r="G255" t="n">
+        <v>20756.98471103632</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -6074,6 +6841,9 @@
       <c r="F256" t="n">
         <v>50212088965</v>
       </c>
+      <c r="G256" t="n">
+        <v>21160.35083796474</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -6096,6 +6866,9 @@
       <c r="F257" t="n">
         <v>51091116622</v>
       </c>
+      <c r="G257" t="n">
+        <v>20944.43988628605</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -6118,6 +6891,9 @@
       <c r="F258" t="n">
         <v>37872380889</v>
       </c>
+      <c r="G258" t="n">
+        <v>20768.60237565204</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -6140,6 +6916,9 @@
       <c r="F259" t="n">
         <v>36389011503</v>
       </c>
+      <c r="G259" t="n">
+        <v>20501.75451611403</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -6162,6 +6941,9 @@
       <c r="F260" t="n">
         <v>30123362273</v>
       </c>
+      <c r="G260" t="n">
+        <v>20319.46188317927</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -6184,6 +6966,9 @@
       <c r="F261" t="n">
         <v>24957448100</v>
       </c>
+      <c r="G261" t="n">
+        <v>20271.4904553532</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -6206,6 +6991,9 @@
       <c r="F262" t="n">
         <v>31254779144</v>
       </c>
+      <c r="G262" t="n">
+        <v>20058.49430635865</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -6228,6 +7016,9 @@
       <c r="F263" t="n">
         <v>40177002624</v>
       </c>
+      <c r="G263" t="n">
+        <v>19929.90295633149</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -6250,6 +7041,9 @@
       <c r="F264" t="n">
         <v>36791346508</v>
       </c>
+      <c r="G264" t="n">
+        <v>19670.12448287362</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -6272,6 +7066,9 @@
       <c r="F265" t="n">
         <v>46363793975</v>
       </c>
+      <c r="G265" t="n">
+        <v>19389.44345981146</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -6294,6 +7091,9 @@
       <c r="F266" t="n">
         <v>41135767926</v>
       </c>
+      <c r="G266" t="n">
+        <v>19395.4702901711</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -6316,6 +7116,9 @@
       <c r="F267" t="n">
         <v>38896078052</v>
       </c>
+      <c r="G267" t="n">
+        <v>19371.01238559707</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -6338,6 +7141,9 @@
       <c r="F268" t="n">
         <v>26149643168</v>
       </c>
+      <c r="G268" t="n">
+        <v>19262.5122188853</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -6360,6 +7166,9 @@
       <c r="F269" t="n">
         <v>23359966112</v>
       </c>
+      <c r="G269" t="n">
+        <v>19147.40857822648</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -6382,6 +7191,9 @@
       <c r="F270" t="n">
         <v>44148798321</v>
       </c>
+      <c r="G270" t="n">
+        <v>19166.22440241986</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -6404,6 +7216,9 @@
       <c r="F271" t="n">
         <v>58571439619</v>
       </c>
+      <c r="G271" t="n">
+        <v>19152.30502056489</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -6426,6 +7241,9 @@
       <c r="F272" t="n">
         <v>53071298734</v>
       </c>
+      <c r="G272" t="n">
+        <v>19220.90894120492</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -6448,6 +7266,9 @@
       <c r="F273" t="n">
         <v>41037843771</v>
       </c>
+      <c r="G273" t="n">
+        <v>19308.94440121619</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -6470,6 +7291,9 @@
       <c r="F274" t="n">
         <v>43975248085</v>
       </c>
+      <c r="G274" t="n">
+        <v>19339.65556653714</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -6492,6 +7316,9 @@
       <c r="F275" t="n">
         <v>18719537670</v>
       </c>
+      <c r="G275" t="n">
+        <v>19332.76560068411</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -6514,6 +7341,9 @@
       <c r="F276" t="n">
         <v>20765955327</v>
       </c>
+      <c r="G276" t="n">
+        <v>19260.60105598183</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -6536,6 +7366,9 @@
       <c r="F277" t="n">
         <v>30484729489</v>
       </c>
+      <c r="G277" t="n">
+        <v>19351.34581151763</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -6558,6 +7391,9 @@
       <c r="F278" t="n">
         <v>35887278685</v>
       </c>
+      <c r="G278" t="n">
+        <v>19597.72029613822</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -6580,6 +7416,9 @@
       <c r="F279" t="n">
         <v>33223790572</v>
       </c>
+      <c r="G279" t="n">
+        <v>19738.46942132241</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -6602,6 +7441,9 @@
       <c r="F280" t="n">
         <v>34711412966</v>
       </c>
+      <c r="G280" t="n">
+        <v>19792.71290583556</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -6624,6 +7466,9 @@
       <c r="F281" t="n">
         <v>29227315390</v>
       </c>
+      <c r="G281" t="n">
+        <v>19731.24708172042</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -6646,6 +7491,9 @@
       <c r="F282" t="n">
         <v>16437423167</v>
       </c>
+      <c r="G282" t="n">
+        <v>19652.57740113407</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -6668,6 +7516,9 @@
       <c r="F283" t="n">
         <v>16837262532</v>
       </c>
+      <c r="G283" t="n">
+        <v>19601.03949616305</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -6690,6 +7541,9 @@
       <c r="F284" t="n">
         <v>27425022774</v>
       </c>
+      <c r="G284" t="n">
+        <v>19486.15071587229</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -6712,6 +7566,9 @@
       <c r="F285" t="n">
         <v>28711532910</v>
       </c>
+      <c r="G285" t="n">
+        <v>19377.46752909171</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -6734,6 +7591,9 @@
       <c r="F286" t="n">
         <v>24950173846</v>
       </c>
+      <c r="G286" t="n">
+        <v>19322.46197494378</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -6756,6 +7616,9 @@
       <c r="F287" t="n">
         <v>44219840004</v>
       </c>
+      <c r="G287" t="n">
+        <v>19337.57255542659</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -6778,6 +7641,9 @@
       <c r="F288" t="n">
         <v>38452356727</v>
       </c>
+      <c r="G288" t="n">
+        <v>19299.59347906994</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -6800,6 +7666,9 @@
       <c r="F289" t="n">
         <v>16192235532</v>
       </c>
+      <c r="G289" t="n">
+        <v>19241.6038007087</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -6822,6 +7691,9 @@
       <c r="F290" t="n">
         <v>17988916650</v>
       </c>
+      <c r="G290" t="n">
+        <v>19248.22628803153</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -6844,6 +7716,9 @@
       <c r="F291" t="n">
         <v>27472552998</v>
       </c>
+      <c r="G291" t="n">
+        <v>19323.85916914865</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -6866,6 +7741,9 @@
       <c r="F292" t="n">
         <v>30580012344</v>
       </c>
+      <c r="G292" t="n">
+        <v>19326.49838076773</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -6888,6 +7766,9 @@
       <c r="F293" t="n">
         <v>22425387184</v>
       </c>
+      <c r="G293" t="n">
+        <v>19279.7575746383</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -6910,6 +7791,9 @@
       <c r="F294" t="n">
         <v>24493974420</v>
       </c>
+      <c r="G294" t="n">
+        <v>19223.25323957248</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -6932,6 +7816,9 @@
       <c r="F295" t="n">
         <v>32459287866</v>
       </c>
+      <c r="G295" t="n">
+        <v>19210.55711717936</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -6954,6 +7841,9 @@
       <c r="F296" t="n">
         <v>16104440957</v>
       </c>
+      <c r="G296" t="n">
+        <v>19209.96520116577</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -6976,6 +7866,9 @@
       <c r="F297" t="n">
         <v>22128794335</v>
       </c>
+      <c r="G297" t="n">
+        <v>19299.22585399933</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -6998,6 +7891,9 @@
       <c r="F298" t="n">
         <v>30202235805</v>
       </c>
+      <c r="G298" t="n">
+        <v>19310.81245690575</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -7020,6 +7916,9 @@
       <c r="F299" t="n">
         <v>47761524910</v>
       </c>
+      <c r="G299" t="n">
+        <v>19507.07369814806</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -7042,6 +7941,9 @@
       <c r="F300" t="n">
         <v>58895950537</v>
       </c>
+      <c r="G300" t="n">
+        <v>19822.91562517354</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -7064,6 +7966,9 @@
       <c r="F301" t="n">
         <v>49625110402</v>
       </c>
+      <c r="G301" t="n">
+        <v>19938.64570325516</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -7086,6 +7991,9 @@
       <c r="F302" t="n">
         <v>43994715910</v>
       </c>
+      <c r="G302" t="n">
+        <v>20102.82216806637</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -7108,6 +8016,9 @@
       <c r="F303" t="n">
         <v>40369840645</v>
       </c>
+      <c r="G303" t="n">
+        <v>20281.73576667478</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -7130,6 +8041,9 @@
       <c r="F304" t="n">
         <v>31486345556</v>
       </c>
+      <c r="G304" t="n">
+        <v>20370.20270391233</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -7152,6 +8066,9 @@
       <c r="F305" t="n">
         <v>45668466815</v>
       </c>
+      <c r="G305" t="n">
+        <v>20401.59538730925</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -7174,6 +8091,9 @@
       <c r="F306" t="n">
         <v>39819303159</v>
       </c>
+      <c r="G306" t="n">
+        <v>20422.51489985694</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -7196,6 +8116,9 @@
       <c r="F307" t="n">
         <v>55552169483</v>
       </c>
+      <c r="G307" t="n">
+        <v>20356.7621514552</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -7218,6 +8141,9 @@
       <c r="F308" t="n">
         <v>43228750179</v>
       </c>
+      <c r="G308" t="n">
+        <v>20320.0686839039</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -7240,6 +8166,9 @@
       <c r="F309" t="n">
         <v>64072727950</v>
       </c>
+      <c r="G309" t="n">
+        <v>20526.85913011543</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -7262,6 +8191,9 @@
       <c r="F310" t="n">
         <v>37846047609</v>
       </c>
+      <c r="G310" t="n">
+        <v>20715.81719914907</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -7284,6 +8216,9 @@
       <c r="F311" t="n">
         <v>35082693210</v>
       </c>
+      <c r="G311" t="n">
+        <v>20768.48448139305</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -7306,6 +8241,9 @@
       <c r="F312" t="n">
         <v>53510852236</v>
       </c>
+      <c r="G312" t="n">
+        <v>20727.06746260729</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -7328,6 +8266,9 @@
       <c r="F313" t="n">
         <v>118992465607</v>
       </c>
+      <c r="G313" t="n">
+        <v>20180.61846804922</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -7350,6 +8291,9 @@
       <c r="F314" t="n">
         <v>102905151606</v>
       </c>
+      <c r="G314" t="n">
+        <v>19105.65891939629</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -7372,6 +8316,9 @@
       <c r="F315" t="n">
         <v>83202283721</v>
       </c>
+      <c r="G315" t="n">
+        <v>18725.93706064097</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -7394,6 +8341,9 @@
       <c r="F316" t="n">
         <v>55871616488</v>
       </c>
+      <c r="G316" t="n">
+        <v>18303.02603766823</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -7416,6 +8366,9 @@
       <c r="F317" t="n">
         <v>29717699419</v>
       </c>
+      <c r="G317" t="n">
+        <v>17927.06591496992</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -7438,6 +8391,9 @@
       <c r="F318" t="n">
         <v>27209183682</v>
       </c>
+      <c r="G318" t="n">
+        <v>17533.64074482119</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -7460,6 +8416,9 @@
       <c r="F319" t="n">
         <v>49630243054</v>
       </c>
+      <c r="G319" t="n">
+        <v>17304.78036330339</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -7482,6 +8441,9 @@
       <c r="F320" t="n">
         <v>36599436183</v>
       </c>
+      <c r="G320" t="n">
+        <v>17199.73859279004</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -7504,6 +8466,9 @@
       <c r="F321" t="n">
         <v>33925512989</v>
       </c>
+      <c r="G321" t="n">
+        <v>17067.16380787378</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -7526,6 +8491,9 @@
       <c r="F322" t="n">
         <v>27868914022</v>
       </c>
+      <c r="G322" t="n">
+        <v>16972.25225043658</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -7548,6 +8516,9 @@
       <c r="F323" t="n">
         <v>26862218609</v>
       </c>
+      <c r="G323" t="n">
+        <v>16903.63352376494</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -7570,6 +8541,9 @@
       <c r="F324" t="n">
         <v>16106223492</v>
       </c>
+      <c r="G324" t="n">
+        <v>16855.61186157371</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -7592,6 +8566,9 @@
       <c r="F325" t="n">
         <v>21313378652</v>
       </c>
+      <c r="G325" t="n">
+        <v>16714.66690399278</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -7614,6 +8591,9 @@
       <c r="F326" t="n">
         <v>37429485518</v>
       </c>
+      <c r="G326" t="n">
+        <v>16482.82122291646</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -7636,6 +8616,9 @@
       <c r="F327" t="n">
         <v>30726828760</v>
       </c>
+      <c r="G327" t="n">
+        <v>16409.55829999984</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -7658,6 +8641,9 @@
       <c r="F328" t="n">
         <v>32958875628</v>
       </c>
+      <c r="G328" t="n">
+        <v>16459.84548281238</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -7680,6 +8666,9 @@
       <c r="F329" t="n">
         <v>26129037414</v>
       </c>
+      <c r="G329" t="n">
+        <v>16496.00032304679</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -7702,6 +8691,9 @@
       <c r="F330" t="n">
         <v>18678255976</v>
       </c>
+      <c r="G330" t="n">
+        <v>16502.46069150384</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -7724,6 +8716,9 @@
       <c r="F331" t="n">
         <v>18000008764</v>
       </c>
+      <c r="G331" t="n">
+        <v>16492.91583112788</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -7746,6 +8741,9 @@
       <c r="F332" t="n">
         <v>20443898509</v>
       </c>
+      <c r="G332" t="n">
+        <v>16480.84361162716</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -7768,6 +8766,9 @@
       <c r="F333" t="n">
         <v>27743025156</v>
       </c>
+      <c r="G333" t="n">
+        <v>16414.96327512662</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -7790,6 +8791,9 @@
       <c r="F334" t="n">
         <v>23581685468</v>
       </c>
+      <c r="G334" t="n">
+        <v>16422.46806181372</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -7812,6 +8816,9 @@
       <c r="F335" t="n">
         <v>29523576583</v>
       </c>
+      <c r="G335" t="n">
+        <v>16608.99264792279</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -7834,6 +8841,9 @@
       <c r="F336" t="n">
         <v>22895392882</v>
       </c>
+      <c r="G336" t="n">
+        <v>16698.52768906709</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -7856,6 +8866,9 @@
       <c r="F337" t="n">
         <v>19539705127</v>
       </c>
+      <c r="G337" t="n">
+        <v>16796.06080586282</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -7878,6 +8891,9 @@
       <c r="F338" t="n">
         <v>16217776704</v>
       </c>
+      <c r="G338" t="n">
+        <v>16824.10468642836</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -7900,6 +8916,9 @@
       <c r="F339" t="n">
         <v>16824520830</v>
       </c>
+      <c r="G339" t="n">
+        <v>16900.70009685252</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -7922,6 +8941,9 @@
       <c r="F340" t="n">
         <v>22209086834</v>
       </c>
+      <c r="G340" t="n">
+        <v>16919.23161560814</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -7944,6 +8966,9 @@
       <c r="F341" t="n">
         <v>19889922369</v>
       </c>
+      <c r="G341" t="n">
+        <v>16961.79968826861</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -7966,6 +8991,9 @@
       <c r="F342" t="n">
         <v>19675404389</v>
       </c>
+      <c r="G342" t="n">
+        <v>16933.38150448271</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -7988,6 +9016,9 @@
       <c r="F343" t="n">
         <v>20496603770</v>
       </c>
+      <c r="G343" t="n">
+        <v>17008.40478070578</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -8010,6 +9041,9 @@
       <c r="F344" t="n">
         <v>20328426366</v>
       </c>
+      <c r="G344" t="n">
+        <v>17039.59167146683</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -8032,6 +9066,9 @@
       <c r="F345" t="n">
         <v>12706781969</v>
       </c>
+      <c r="G345" t="n">
+        <v>17061.87490594388</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -8054,6 +9091,9 @@
       <c r="F346" t="n">
         <v>14122486832</v>
       </c>
+      <c r="G346" t="n">
+        <v>17072.45451930166</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -8076,6 +9116,9 @@
       <c r="F347" t="n">
         <v>19617581341</v>
       </c>
+      <c r="G347" t="n">
+        <v>17105.95026447625</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -8098,6 +9141,9 @@
       <c r="F348" t="n">
         <v>26634741631</v>
       </c>
+      <c r="G348" t="n">
+        <v>17274.79228820094</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -8120,6 +9166,9 @@
       <c r="F349" t="n">
         <v>25534481470</v>
       </c>
+      <c r="G349" t="n">
+        <v>17410.00681380695</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -8142,6 +9191,9 @@
       <c r="F350" t="n">
         <v>20964448341</v>
       </c>
+      <c r="G350" t="n">
+        <v>17398.72141894897</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -8164,6 +9216,9 @@
       <c r="F351" t="n">
         <v>24031608960</v>
       </c>
+      <c r="G351" t="n">
+        <v>17210.91215796173</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -8186,6 +9241,9 @@
       <c r="F352" t="n">
         <v>14463581825</v>
       </c>
+      <c r="G352" t="n">
+        <v>17106.95706769005</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -8208,6 +9266,9 @@
       <c r="F353" t="n">
         <v>10924354698</v>
       </c>
+      <c r="G353" t="n">
+        <v>17019.71194139254</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -8230,6 +9291,9 @@
       <c r="F354" t="n">
         <v>17221074814</v>
       </c>
+      <c r="G354" t="n">
+        <v>16874.7038779194</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -8252,6 +9316,9 @@
       <c r="F355" t="n">
         <v>22722096615</v>
       </c>
+      <c r="G355" t="n">
+        <v>16882.60408031455</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -8274,6 +9341,9 @@
       <c r="F356" t="n">
         <v>14882945045</v>
       </c>
+      <c r="G356" t="n">
+        <v>16866.33684929842</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -8296,6 +9366,9 @@
       <c r="F357" t="n">
         <v>16441573050</v>
       </c>
+      <c r="G357" t="n">
+        <v>16857.33808619256</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -8318,6 +9391,9 @@
       <c r="F358" t="n">
         <v>15329265213</v>
       </c>
+      <c r="G358" t="n">
+        <v>16842.24184589442</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -8340,6 +9416,9 @@
       <c r="F359" t="n">
         <v>9744636213</v>
       </c>
+      <c r="G359" t="n">
+        <v>16843.62034926457</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -8362,6 +9441,9 @@
       <c r="F360" t="n">
         <v>11656379938</v>
       </c>
+      <c r="G360" t="n">
+        <v>16843.21184397968</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -8384,6 +9466,9 @@
       <c r="F361" t="n">
         <v>11886957804</v>
       </c>
+      <c r="G361" t="n">
+        <v>16862.36005485976</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -8406,6 +9491,9 @@
       <c r="F362" t="n">
         <v>15748580239</v>
       </c>
+      <c r="G362" t="n">
+        <v>16826.06349817607</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -8428,6 +9516,9 @@
       <c r="F363" t="n">
         <v>17005713920</v>
       </c>
+      <c r="G363" t="n">
+        <v>16757.6906900383</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -8450,6 +9541,9 @@
       <c r="F364" t="n">
         <v>14472237479</v>
       </c>
+      <c r="G364" t="n">
+        <v>16728.85346674747</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -8471,6 +9565,9 @@
       </c>
       <c r="F365" t="n">
         <v>15929162910</v>
+      </c>
+      <c r="G365" t="n">
+        <v>16697.28658443561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>